<commit_message>
add more simple plotting tutorials
</commit_message>
<xml_diff>
--- a/data/ratings_climateactiontracker.xlsx
+++ b/data/ratings_climateactiontracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/c4021106/Dropbox/teach/r-tutorial-beginner/RTutorial/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisalechner/Dropbox/teach/r-tutorial-beginner/RTutorial/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31C8289-3AA7-BF4B-8AD1-C2CFECFB3D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74228AC-BB73-654A-A697-112A5F7AF3AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="11140" windowWidth="26340" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>Russian Federation</t>
   </si>
   <si>
-    <t>Sangapore</t>
-  </si>
-  <si>
     <t>Thailand</t>
   </si>
   <si>
@@ -157,6 +154,9 @@
   </si>
   <si>
     <t>rating</t>
+  </si>
+  <si>
+    <t>Singapore</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -490,7 +490,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -511,7 +511,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -527,7 +527,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -535,7 +535,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -543,258 +543,258 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>